<commit_message>
Resolved Play Store descriptions issue by handling span elements outside and inside description blocks.
Google Search Automation project

- Implemented Selenium automation to perform Google searches.
- Extracted titles, URLs, and descriptions from search results.
- Resolved Play Store descriptions issue by handling span elements outside and inside description blocks.
- Added Excel export functionality for search results.
- Optimized code structure and organization for better maintainability.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Termo de Busca</t>
   </si>
@@ -35,7 +35,7 @@
     <t>https://www.pokemon.com/us</t>
   </si>
   <si>
-    <t>Featured Pokémon · Lokix 920 · Boltund 836 · Archaludon 1018 · Porygon2 233 · Pignite 499 · Darumaka 554 · Hatenna 856 · Vivillon 666.</t>
+    <t>What's New This Week · Dragon-Type Pokémon Soar over Pokéween · Scarlet &amp; Violet—Stellar Crown Triple Play Deck Strategy · Live, Laugh, Scare with Pokémon ...</t>
   </si>
   <si>
     <t>Pokémon</t>
@@ -65,13 +65,13 @@
     <t>Watch Pokémon Video Game, Trading Card Game, and Animation content, along with special features, and event highlights right here on the official Pokémon ...</t>
   </si>
   <si>
-    <t>Pokémon - Toys, Games &amp; Trading Cards</t>
-  </si>
-  <si>
-    <t>https://www.smythstoys.com/ie/en-ie/brand/pokemon/c/pokemon-brand</t>
-  </si>
-  <si>
-    <t>Buy Pokémon toys, games and trading cards at Smyths Toys Ireland! FREE DELIVERY over €25 ✔️ Click &amp; Collect available.</t>
+    <t>Pokemon - Pokémon</t>
+  </si>
+  <si>
+    <t>https://twitter.com/pokemon</t>
+  </si>
+  <si>
+    <t>Infernape with the Mightiest Mark is now appearing in black crystal Tera Raid Battles throughout #PokemonScarletViolet! Work together with friends to topple ...</t>
   </si>
   <si>
     <t>Minecraft</t>
@@ -98,7 +98,16 @@
     <t>https://play.google.com/store/apps/details?id=com.mojang.minecraftpe&amp;hl=en_US</t>
   </si>
   <si>
-    <t>há 3 dias —</t>
+    <t>— Explore and craft your way through a completely open world where you can play with friends, build a city, start a farm, mine deep into the ...</t>
+  </si>
+  <si>
+    <t>Minecraft - PS4 Games</t>
+  </si>
+  <si>
+    <t>https://www.playstation.com/en-ie/games/minecraft/</t>
+  </si>
+  <si>
+    <t>Team up or go solo and triumph over waves of hostile mobs, build with new blocks, harness auto-crafting, battle the breeze, unlock the vault, and more.</t>
   </si>
   <si>
     <t>r/Minecraft</t>
@@ -110,10 +119,52 @@
     <t>r/Minecraft: Minecraft community on Reddit.</t>
   </si>
   <si>
-    <t>https://www.youtube.com/minecraft</t>
-  </si>
-  <si>
-    <t>Our monthly news show around all things Minecraft! Get the latest news about all our games from Mojang Studios!</t>
+    <t>Burguer</t>
+  </si>
+  <si>
+    <t>Burger King</t>
+  </si>
+  <si>
+    <t>https://www.burgerking.pt/pt/</t>
+  </si>
+  <si>
+    <t>Nearby restaurant! Free delivery. Free Delivery. In orders up to 20€. Order now!</t>
+  </si>
+  <si>
+    <t>Burger King®</t>
+  </si>
+  <si>
+    <t>https://www.burgerking.com.br/</t>
+  </si>
+  <si>
+    <t>Baixe nosso App e tenha o BK na palma da sua mão! · Centro de preferências de privacidade.</t>
+  </si>
+  <si>
+    <t>Home - Burger KingBurger King | HUNGRY? WE GOT YOU</t>
+  </si>
+  <si>
+    <t>https://www.whopper.ie/</t>
+  </si>
+  <si>
+    <t>Gourmet Kings · Veggie &amp; Plant-based Kings · Texas Bacon Lovers · Sweet Treats.</t>
+  </si>
+  <si>
+    <t>Bilbo Burguer ®️ (@bilboburguer)</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/bilboburguer/</t>
+  </si>
+  <si>
+    <t>CUPOM PRIMEIRA COMPRA: PRIMEIRAVEZ 🎟️ R. José Moreira, Itinga em Lauro de Freitas Pedindo no site chega mais rápido ⇊ Link para pedidos abaixo.</t>
+  </si>
+  <si>
+    <t>'O' Burguer</t>
+  </si>
+  <si>
+    <t>http://www.oburguer.com.br/</t>
+  </si>
+  <si>
+    <t>'O' Burguer é muito mais do que uma simples hamburgueria. Inspirada pela ciência e pela criatividade gastronômica, cada um de nossos produtos é uma experiência ...</t>
   </si>
   <si>
     <t>League of Legends</t>
@@ -176,7 +227,16 @@
     <t>https://play.google.com/store/apps/details?id=com.riotgames.league.wildrift</t>
   </si>
   <si>
-    <t>24 de jul. de 2024 —</t>
+    <t>— Enjoy fast-paced MOBA combat, real-time strategy, smooth controls, and diverse 5v5 gameplay. Team up with friends, lock in your champion, and ...</t>
+  </si>
+  <si>
+    <t>League of Legends: Wild Rift</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/wildrift</t>
+  </si>
+  <si>
+    <t>Dive into League of Legends: Wild Rift: the skills-and-strategy 5v5 MOBA experience of League of Legends by Riot Games, now built from the ground up for ...</t>
   </si>
   <si>
     <t>WildRiftFire: Wild Rift Builds &amp; Guides</t>
@@ -188,19 +248,13 @@
     <t>Find the best build guide for Wild Rift on WildRiftFire. Learn which items, runes, and summoner spells to take on each champion in Wild Rift, as well as how ...</t>
   </si>
   <si>
-    <t>League of Legends: Wild Rift</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/c/wildrift</t>
-  </si>
-  <si>
-    <t>Dive into League of Legends: Wild Rift: the skills-and-strategy 5v5 MOBA experience of League of Legends by Riot Games, now built from the ground up for ...</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/League_of_Legends:_Wild_Rift</t>
-  </si>
-  <si>
-    <t>League of Legends: Wild Rift (abbreviated League: WR or simply Wild Rift) is a multiplayer online battle arena mobile game developed and published by Riot ...</t>
+    <t>League of Legends: Wild Rift (@wildrift) ...</t>
+  </si>
+  <si>
+    <t>https://twitter.com/wildrift</t>
+  </si>
+  <si>
+    <t>Official account of League of Legends: Wild Rift, your favorite mobile MOBA from @riotgames.</t>
   </si>
 </sst>
 </file>
@@ -247,7 +301,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -398,153 +452,223 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>